<commit_message>
Correção da planilha de Ordem 2 da falha FSiEOS (2 valores médios iguais para N = 8 na planilha da revisão 30, trocar SOMA por MÍN ou MAX ou ainda alguma outra função que escolha um dos valores médios).
</commit_message>
<xml_diff>
--- a/planilhas/deteccao/FSiEOS/O2.xlsx
+++ b/planilhas/deteccao/FSiEOS/O2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="19320" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="19320" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="N8" sheetId="16" r:id="rId1"/>
@@ -680,8 +680,8 @@
   <sheetPr codeName="Plan3"/>
   <dimension ref="B2:J45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:I29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,36 +1600,36 @@
         <v>37</v>
       </c>
       <c r="D43" s="11" t="str">
-        <f ca="1">IF(SUM($G$34:$G$39) &lt;&gt; 0, CONCATENATE("$C$",SUM($G$34:$G$39)), "" )</f>
-        <v>$C$70</v>
+        <f ca="1">IF(SUM($G$34:$G$39) &lt;&gt; 0, CONCATENATE("$C$",MIN($G$34:$G$39)), "" )</f>
+        <v>$C$34</v>
       </c>
       <c r="E43" s="11">
         <f ca="1">INDIRECT(D43)</f>
-        <v>0</v>
+        <v>23994</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
       <c r="C44" s="28"/>
       <c r="D44" s="11" t="str">
-        <f ca="1">IF(SUM($G$34:$G$39) &lt;&gt; 0, CONCATENATE("$D$",SUM($G$34:$G$39)), "" )</f>
-        <v>$D$70</v>
+        <f ca="1">IF(SUM($G$34:$G$39) &lt;&gt; 0, CONCATENATE("$D$",MIN($G$34:$G$39)), "" )</f>
+        <v>$D$34</v>
       </c>
       <c r="E44" s="11">
         <f ca="1">INDIRECT(D44)</f>
-        <v>0</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="27"/>
       <c r="C45" s="28"/>
       <c r="D45" s="11" t="str">
-        <f ca="1">IF(SUM($G$34:$G$39) &lt;&gt; 0, CONCATENATE("$E$",SUM($G$34:$G$39)), "" )</f>
-        <v>$E$70</v>
+        <f ca="1">IF(SUM($G$34:$G$39) &lt;&gt; 0, CONCATENATE("$E$",MIN($G$34:$G$39)), "" )</f>
+        <v>$E$34</v>
       </c>
       <c r="E45" s="11">
         <f ca="1">INDIRECT(D45)</f>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
     </row>
   </sheetData>
@@ -2644,7 +2644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29:I29"/>
     </sheetView>
   </sheetViews>
@@ -3680,23 +3680,23 @@
       </c>
       <c r="D5" s="11">
         <f ca="1">'N8'!$E43</f>
-        <v>0</v>
+        <v>23994</v>
       </c>
       <c r="E5" s="11">
         <f ca="1">'N8'!$E44</f>
-        <v>0</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="F5" s="11">
         <f ca="1">'N8'!$E45</f>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="G5" s="11">
         <f ca="1">SUM(E5:F5)</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="15">
+        <v>6</v>
+      </c>
+      <c r="I5" s="15" t="str">
         <f ca="1">IF(G5=MIN($G$5:$G$7),CELL("lin",G5),"")</f>
-        <v>5</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -3723,9 +3723,9 @@
         <f t="shared" ref="G6:G7" ca="1" si="0">SUM(E6:F6)</f>
         <v>4.3333333333333339</v>
       </c>
-      <c r="I6" s="15" t="str">
+      <c r="I6" s="15">
         <f t="shared" ref="I6:I7" ca="1" si="1">IF(G6=MIN($G$5:$G$7),CELL("lin",G6),"")</f>
-        <v/>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -3790,27 +3790,27 @@
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <f ca="1">INDIRECT(CONCATENATE("$B$",SUM($I$5:$I$7)))</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C11" s="11">
         <f ca="1">INDIRECT(CONCATENATE("$C$",SUM($I$5:$I$7)))</f>
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D11" s="11">
         <f ca="1">INDIRECT(CONCATENATE("$D$",SUM($I$5:$I$7)))</f>
-        <v>0</v>
+        <v>23995.666666666668</v>
       </c>
       <c r="E11" s="11">
         <f ca="1">INDIRECT(CONCATENATE("$E$",SUM($I$5:$I$7)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="11">
         <f ca="1">INDIRECT(CONCATENATE("$F$",SUM($I$5:$I$7)))</f>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="G11" s="11">
         <f ca="1">INDIRECT(CONCATENATE("$G$",SUM($I$5:$I$7)))</f>
-        <v>0</v>
+        <v>4.3333333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>